<commit_message>
updated Excel Weighting Test
</commit_message>
<xml_diff>
--- a/reports/WeightingCalcsTest.xlsx
+++ b/reports/WeightingCalcsTest.xlsx
@@ -24,7 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>UNW</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -107,6 +114,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Unweighted</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Signals</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -195,11 +231,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="526651896"/>
-        <c:axId val="526656208"/>
+        <c:axId val="608674272"/>
+        <c:axId val="608674664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526651896"/>
+        <c:axId val="608674272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -241,7 +277,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526656208"/>
+        <c:crossAx val="608674664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -249,7 +285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526656208"/>
+        <c:axId val="608674664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,7 +336,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526651896"/>
+        <c:crossAx val="608674272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -364,6 +400,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Weighted Signals</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -452,11 +513,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="691837864"/>
-        <c:axId val="691837080"/>
+        <c:axId val="608675448"/>
+        <c:axId val="608675840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="691837864"/>
+        <c:axId val="608675448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -498,7 +559,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="691837080"/>
+        <c:crossAx val="608675840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -506,7 +567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="691837080"/>
+        <c:axId val="608675840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +618,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="691837864"/>
+        <c:crossAx val="608675448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -621,6 +682,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Using Normalized Scale</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -661,6 +751,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UNW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -673,27 +774,79 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$F$10</c:f>
+              <c:f>Sheet1!$B$24:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>48.84545</c:v>
+                  <c:v>0.57343922480345</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.468090000000004</c:v>
+                  <c:v>2.7629864944007675E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.945650000000001</c:v>
+                  <c:v>0.11556924059843461</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.863160000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.689660000000003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.60577</c:v>
+                  <c:v>0.38746020196283731</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$25:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.43872146643566712</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6253037129630575E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0612142316992213E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26889218862616349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -709,17 +862,16 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="526652288"/>
-        <c:axId val="526651112"/>
+        <c:axId val="612426152"/>
+        <c:axId val="612429288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526652288"/>
+        <c:axId val="612426152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -756,7 +908,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526651112"/>
+        <c:crossAx val="612429288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -764,7 +916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526651112"/>
+        <c:axId val="612429288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -815,7 +967,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526652288"/>
+        <c:crossAx val="612426152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -827,6 +979,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2497,16 +2681,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2527,16 +2711,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2557,20 +2741,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>395287</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2851,10 +3035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2862,7 +3046,7 @@
     <col min="1" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>-51.15455</v>
       </c>
@@ -2881,8 +3065,12 @@
       <c r="F1" s="1">
         <v>-56.39423</v>
       </c>
+      <c r="J1">
+        <f>(MAX(A1:F1)-MIN(A1:F1))/MIN(A1:F1)</f>
+        <v>-0.41856124928205679</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>1/A1</f>
         <v>-1.9548603203429608E-2</v>
@@ -2912,7 +3100,7 @@
         <v>-0.10833096916076328</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2/$G$2</f>
         <v>0.18045258299516789</v>
@@ -2937,57 +3125,75 @@
         <f t="shared" si="1"/>
         <v>0.16368643883346692</v>
       </c>
+      <c r="J4">
+        <f>(MAX(A4:F4)-MIN(A4:F4))/MIN(A4:F4)</f>
+        <v>0.71987160946054907</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>A1*A4</f>
-        <v>-9.2309706794554653</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ref="B6:F6" si="2">B1*B4</f>
-        <v>-9.2309706794554653</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="2"/>
-        <v>-9.2309706794554653</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="2"/>
-        <v>-9.2309706794554653</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>-9.2309706794554653</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>-9.2309706794554653</v>
-      </c>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <f>A1+100</f>
-        <v>48.84545</v>
-      </c>
-      <c r="B10" s="1">
-        <f t="shared" ref="B10:F10" si="3">B1+100</f>
-        <v>33.468090000000004</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" si="3"/>
-        <v>35.945650000000001</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="3"/>
-        <v>60.863160000000001</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="3"/>
-        <v>32.689660000000003</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="3"/>
-        <v>43.60577</v>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <f>(A1-MIN($A$1:$F$1))/(MAX($A$1:$F$1)-MIN($A$1:$F$1))</f>
+        <v>0.57343922480345</v>
+      </c>
+      <c r="C24">
+        <f>(B1-MIN($A$1:$F$1))/(MAX($A$1:$F$1)-MIN($A$1:$F$1))</f>
+        <v>2.7629864944007675E-2</v>
+      </c>
+      <c r="D24">
+        <f>(C1-MIN($A$1:$F$1))/(MAX($A$1:$F$1)-MIN($A$1:$F$1))</f>
+        <v>0.11556924059843461</v>
+      </c>
+      <c r="E24">
+        <f>(D1-MIN($A$1:$F$1))/(MAX($A$1:$F$1)-MIN($A$1:$F$1))</f>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f>(E1-MIN($A$1:$F$1))/(MAX($A$1:$F$1)-MIN($A$1:$F$1))</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f>(F1-MIN($A$1:$F$1))/(MAX($A$1:$F$1)-MIN($A$1:$F$1))</f>
+        <v>0.38746020196283731</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <f>(A4-MIN($A$4:$F$4))/(MAX($A$4:$F$4)-MIN($A$4:$F$4))</f>
+        <v>0.43872146643566712</v>
+      </c>
+      <c r="C25">
+        <f>(B4-MIN($A$4:$F$4))/(MAX($A$4:$F$4)-MIN($A$4:$F$4))</f>
+        <v>1.6253037129630575E-2</v>
+      </c>
+      <c r="D25">
+        <f>(C4-MIN($A$4:$F$4))/(MAX($A$4:$F$4)-MIN($A$4:$F$4))</f>
+        <v>7.0612142316992213E-2</v>
+      </c>
+      <c r="E25">
+        <f>(D4-MIN($A$4:$F$4))/(MAX($A$4:$F$4)-MIN($A$4:$F$4))</f>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f>(E4-MIN($A$4:$F$4))/(MAX($A$4:$F$4)-MIN($A$4:$F$4))</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>(F4-MIN($A$4:$F$4))/(MAX($A$4:$F$4)-MIN($A$4:$F$4))</f>
+        <v>0.26889218862616349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>